<commit_message>
autumn 2021 schedule data + additional pref
</commit_message>
<xml_diff>
--- a/data/elm_autumn_2021/Autumn Quarter on-call schedule preference (Responses).xlsx
+++ b/data/elm_autumn_2021/Autumn Quarter on-call schedule preference (Responses).xlsx
@@ -1,26 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/winston/Desktop/Project/schedule-finder/data/elm_autumn_2021/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EDE671-32B2-F648-BDAB-A09A0FCC47B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="43">
   <si>
     <t>Timestamp</t>
   </si>
@@ -88,6 +79,9 @@
     <t>Additional comments</t>
   </si>
   <si>
+    <t>Vivian Yu</t>
+  </si>
+  <si>
     <t>I'm OK with this day (1)</t>
   </si>
   <si>
@@ -136,77 +130,79 @@
     <t>I’m very busy on Friday’s so I would prefer not to be on-call on those days.</t>
   </si>
   <si>
-    <t>Vivian Yu</t>
+    <t>Jasmine Matchawate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I will be out of UW area on November 19 through the morning of November 22nd due to a family obligation, so that is one of the weekends I know of that I will be unavailable. </t>
+  </si>
+  <si>
+    <t>Noah Williams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting 9/18, I have work at around 9 and 10am on saturdays so I'd like to mind my sleep schedule. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-    </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -396,29 +392,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="28" width="21.5" customWidth="1"/>
+    <col customWidth="1" min="1" max="28" width="21.57"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -486,539 +479,675 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2">
       <c r="A2" s="3">
         <v>44448.954615995375</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>38</v>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3">
       <c r="A3" s="3">
-        <v>44448.969886689811</v>
+        <v>44448.96988668981</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="A4" s="3">
         <v>44449.176791736114</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5">
       <c r="A5" s="3">
         <v>44449.354409050924</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6">
       <c r="A6" s="3">
-        <v>44449.367651631939</v>
+        <v>44449.36765163194</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7">
       <c r="A7" s="3">
-        <v>44449.507558888887</v>
+        <v>44449.50755888889</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8">
       <c r="A8" s="3">
         <v>44450.081720682865</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9">
       <c r="A9" s="3">
-        <v>44450.931862662037</v>
+        <v>44450.93186266204</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>44451.4217965162</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="T10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V10" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>44451.97079475694</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>